<commit_message>
P22142 O Update 20230105
</commit_message>
<xml_diff>
--- a/P22142_PC(國巨)/規格/PDA Sqlite table V1.0.0.xlsx
+++ b/P22142_PC(國巨)/規格/PDA Sqlite table V1.0.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="11016" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="11016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="人員基本資料" sheetId="1" r:id="rId1"/>
@@ -1452,10 +1452,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">廠房代號 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Key</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1465,10 +1461,6 @@
   </si>
   <si>
     <t>nvarchar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>廠房名稱</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2976,6 +2968,14 @@
  RB012 nvarchar(11),
  RB013 nvarchar(3)
 )</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">廠房代號 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>廠房名稱</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3530,10 +3530,10 @@
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="G2" s="20" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3699,47 +3699,47 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -3758,8 +3758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -3776,7 +3776,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="G1" s="20" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3808,25 +3808,25 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>908</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>458</v>
       </c>
       <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>459</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>460</v>
       </c>
       <c r="C4" s="6">
         <v>20</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>461</v>
+        <v>909</v>
       </c>
       <c r="E4" s="6"/>
       <c r="G4" s="20"/>
@@ -3869,17 +3869,17 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="G3" s="20" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3906,7 +3906,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
@@ -4037,10 +4037,10 @@
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="G15" s="20" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -4067,7 +4067,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9" t="s">
@@ -4084,7 +4084,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
@@ -4217,7 +4217,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>5</v>
@@ -4226,7 +4226,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="22"/>
@@ -4240,720 +4240,720 @@
         <v>64</v>
       </c>
       <c r="I31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I36" s="22"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I39" s="22"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I40" s="22"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I45" s="22"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I46" s="22"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I48" s="22"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I51" s="22"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I52" s="22"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I53" s="22"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="I56" s="22"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I57" s="22"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="I58" s="22"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I61" s="15"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="I63" s="15"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I64" s="15"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I65" s="15"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="I66" s="15"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I67" s="15"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
@@ -4963,1222 +4963,1222 @@
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -6201,7 +6201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I410"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18:G33"/>
     </sheetView>
   </sheetViews>
@@ -6222,14 +6222,14 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="G3" s="20" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>84</v>
@@ -6256,31 +6256,31 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="G5" s="22"/>
       <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="16" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="E6" s="17"/>
       <c r="G6" s="22"/>
@@ -6291,13 +6291,13 @@
         <v>47</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C7" s="6">
         <v>10</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E7" s="6"/>
       <c r="G7" s="22"/>
@@ -6308,13 +6308,13 @@
         <v>48</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C8" s="6">
         <v>20</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E8" s="6"/>
       <c r="G8" s="22"/>
@@ -6325,13 +6325,13 @@
         <v>49</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C9" s="6">
         <v>10</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E9" s="6"/>
       <c r="G9" s="22"/>
@@ -6342,13 +6342,13 @@
         <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C10" s="6">
         <v>20</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="14"/>
@@ -6360,16 +6360,16 @@
         <v>51</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="G11" s="22"/>
       <c r="I11" s="20"/>
@@ -6379,32 +6379,32 @@
         <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C12" s="6">
         <v>20</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="G12" s="22"/>
       <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C13" s="9">
         <v>10</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E13" s="9"/>
       <c r="G13" s="22"/>
@@ -6415,13 +6415,13 @@
         <v>53</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E14" s="9"/>
       <c r="G14" s="22"/>
@@ -6429,16 +6429,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C15" s="9">
         <v>10</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E15" s="9"/>
       <c r="G15" s="22"/>
@@ -6449,14 +6449,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="G18" s="20" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -6467,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>3</v>
@@ -6479,17 +6479,17 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="G20" s="22"/>
     </row>
@@ -6498,25 +6498,25 @@
         <v>54</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="16" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E21" s="17"/>
       <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="16" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E22" s="17"/>
       <c r="G22" s="22"/>
@@ -6526,13 +6526,13 @@
         <v>55</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C23" s="6">
         <v>10</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E23" s="6"/>
       <c r="G23" s="22"/>
@@ -6542,13 +6542,13 @@
         <v>56</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C24" s="6">
         <v>20</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E24" s="6"/>
       <c r="G24" s="22"/>
@@ -6558,13 +6558,13 @@
         <v>57</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C25" s="13">
         <v>10</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E25" s="6"/>
       <c r="G25" s="22"/>
@@ -6574,13 +6574,13 @@
         <v>58</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="22"/>
@@ -6590,13 +6590,13 @@
         <v>59</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C27" s="10">
         <v>10</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E27" s="6"/>
       <c r="G27" s="22"/>
@@ -6606,13 +6606,13 @@
         <v>60</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C28" s="6">
         <v>40</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E28" s="6"/>
       <c r="G28" s="22"/>
@@ -6622,61 +6622,61 @@
         <v>61</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C29" s="6">
         <v>40</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E29" s="6"/>
       <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C30" s="12">
         <v>10</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E30" s="9"/>
       <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C31" s="12">
         <v>11</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E31" s="9"/>
       <c r="G31" s="22"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C32" s="12">
         <v>3</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E32" s="9"/>
       <c r="G32" s="22"/>
@@ -6691,32 +6691,32 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>